<commit_message>
restructure for DBServer fixed bugs for Lua's interfaces
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel/Server.xlsx
+++ b/_Out/NFDataCfg/Excel/Server.xlsx
@@ -186,13 +186,13 @@
     <t>LoginServer</t>
   </si>
   <si>
-    <t>AIServer_1</t>
+    <t>DBServer_1</t>
   </si>
   <si>
     <t>8</t>
   </si>
   <si>
-    <t>AIServer</t>
+    <t>DBServer</t>
   </si>
   <si>
     <t>TutorialServer_1</t>
@@ -211,10 +211,10 @@
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -239,6 +239,13 @@
       <sz val="11"/>
       <name val="宋体"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -256,98 +263,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -361,6 +279,51 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -368,9 +331,46 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -384,19 +384,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="宋体"/>
-      <charset val="134"/>
     </font>
   </fonts>
   <fills count="35">
@@ -420,187 +413,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -726,6 +719,15 @@
       </top>
       <bottom style="medium">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -748,8 +750,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -798,8 +800,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -818,29 +820,20 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -850,130 +843,130 @@
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1418,7 +1411,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="J14" sqref="J14"/>
+      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>

</xml_diff>

<commit_message>
actor component and the callback function now supported lambda
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel/Server.xlsx
+++ b/_Out/NFDataCfg/Excel/Server.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21495" windowHeight="9930" tabRatio="990"/>
+    <workbookView windowWidth="21495" windowHeight="10335" tabRatio="990"/>
   </bookViews>
   <sheets>
     <sheet name="Property1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51">
   <si>
     <t>Id</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>Area</t>
+  </si>
+  <si>
+    <t>Cell</t>
   </si>
   <si>
     <t>WebPort</t>
@@ -209,10 +212,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -250,6 +253,59 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -263,6 +319,74 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -270,127 +394,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -413,19 +416,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -437,163 +596,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -750,6 +753,30 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
@@ -772,16 +799,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -796,177 +823,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1406,12 +1409,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
+      <selection pane="bottomLeft" activeCell="J11" sqref="J11:J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1424,10 +1427,10 @@
     <col min="6" max="6" width="15.4"/>
     <col min="7" max="7" width="23"/>
     <col min="8" max="8" width="9.4"/>
-    <col min="9" max="1025" width="8.6"/>
+    <col min="9" max="1026" width="8.6"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="27" spans="1:10">
+    <row r="1" s="1" customFormat="1" ht="27" spans="1:11">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1458,42 +1461,48 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" s="2" customFormat="1" spans="1:10">
+    <row r="2" s="2" customFormat="1" spans="1:11">
       <c r="A2" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>10</v>
-      </c>
       <c r="E2" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="9" t="s">
-        <v>10</v>
-      </c>
       <c r="H2" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="3" s="2" customFormat="1" spans="1:10">
+    <row r="3" s="2" customFormat="1" spans="1:11">
       <c r="A3" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" s="9">
         <v>0</v>
@@ -1522,10 +1531,13 @@
       <c r="J3" s="9">
         <v>0</v>
       </c>
+      <c r="K3" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" s="2" customFormat="1" spans="1:10">
+    <row r="4" s="2" customFormat="1" spans="1:11">
       <c r="A4" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" s="9">
         <v>0</v>
@@ -1554,10 +1566,13 @@
       <c r="J4" s="9">
         <v>0</v>
       </c>
+      <c r="K4" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" s="2" customFormat="1" spans="1:10">
+    <row r="5" s="2" customFormat="1" spans="1:11">
       <c r="A5" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5" s="9">
         <v>0</v>
@@ -1586,10 +1601,13 @@
       <c r="J5" s="9">
         <v>0</v>
       </c>
+      <c r="K5" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" s="2" customFormat="1" spans="1:10">
+    <row r="6" s="2" customFormat="1" spans="1:11">
       <c r="A6" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6" s="9">
         <v>0</v>
@@ -1618,10 +1636,13 @@
       <c r="J6" s="9">
         <v>0</v>
       </c>
+      <c r="K6" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" s="3" customFormat="1" spans="1:10">
+    <row r="7" s="3" customFormat="1" spans="1:11">
       <c r="A7" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" s="9">
         <v>0</v>
@@ -1650,10 +1671,13 @@
       <c r="J7" s="9">
         <v>0</v>
       </c>
+      <c r="K7" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" s="3" customFormat="1" spans="1:10">
+    <row r="8" s="3" customFormat="1" spans="1:11">
       <c r="A8" s="10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B8" s="9">
         <v>0</v>
@@ -1682,10 +1706,13 @@
       <c r="J8" s="9">
         <v>0</v>
       </c>
+      <c r="K8" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" s="3" customFormat="1" spans="1:10">
+    <row r="9" s="3" customFormat="1" spans="1:11">
       <c r="A9" s="10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B9" s="9">
         <v>0</v>
@@ -1714,48 +1741,54 @@
       <c r="J9" s="9">
         <v>0</v>
       </c>
+      <c r="K9" s="9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" s="4" customFormat="1" ht="42.75" spans="1:10">
+    <row r="10" s="4" customFormat="1" ht="42.75" spans="1:11">
       <c r="A10" s="11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J10" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="K10" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:11">
       <c r="A11" s="13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D11">
         <v>5000</v>
@@ -1764,13 +1797,13 @@
         <v>1</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G11">
         <v>16001</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I11">
         <v>1</v>
@@ -1778,16 +1811,19 @@
       <c r="J11">
         <v>0</v>
       </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:11">
       <c r="A12" s="13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D12">
         <v>5000</v>
@@ -1796,13 +1832,13 @@
         <v>1</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G12">
         <v>17001</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I12">
         <v>1</v>
@@ -1810,16 +1846,19 @@
       <c r="J12">
         <v>0</v>
       </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:11">
       <c r="A13" s="13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D13">
         <v>5000</v>
@@ -1828,30 +1867,33 @@
         <v>1</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G13">
         <v>15001</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I13">
         <v>1</v>
       </c>
       <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
         <v>5001</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:11">
       <c r="A14" s="13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D14">
         <v>5000</v>
@@ -1860,30 +1902,33 @@
         <v>1</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G14">
         <v>13001</v>
       </c>
       <c r="H14" s="13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I14">
         <v>1</v>
       </c>
       <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
         <v>3001</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:11">
       <c r="A15" s="14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D15">
         <v>5000</v>
@@ -1892,30 +1937,33 @@
         <v>1</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G15" s="15">
         <v>14001</v>
       </c>
       <c r="H15" s="14" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I15">
         <v>1</v>
       </c>
       <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
         <v>4001</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:11">
       <c r="A16" s="14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D16">
         <v>5000</v>
@@ -1924,13 +1972,13 @@
         <v>1</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G16" s="15">
         <v>18001</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I16">
         <v>1</v>
@@ -1938,16 +1986,19 @@
       <c r="J16">
         <v>0</v>
       </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:11">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D17">
         <v>5000</v>
@@ -1956,18 +2007,21 @@
         <v>1</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G17" s="15">
         <v>14001</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I17">
         <v>1</v>
       </c>
       <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
         <v>0</v>
       </c>
     </row>

</xml_diff>